<commit_message>
Multiple pages were modified. Test cases added to the file. Utilities method curreent date was added
</commit_message>
<xml_diff>
--- a/test_cases/OrangeHRM_test_cases.xlsx
+++ b/test_cases/OrangeHRM_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4eto\pythonProject\orangehrm_demo_framework\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9011776A-A9BB-47F1-A391-82F349B16DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7280423-5896-4C01-9586-FB9ACC44DC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Adding new candidate</t>
   </si>
   <si>
-    <t>Click on add new candidate button and cancel</t>
-  </si>
-  <si>
     <t>Delete last record in the table and verify it was deleted successfully and the number of records decreased by one record</t>
   </si>
   <si>
@@ -165,6 +162,43 @@
   </si>
   <si>
     <t>Edit candidate record</t>
+  </si>
+  <si>
+    <t>Search candidates functionality</t>
+  </si>
+  <si>
+    <t>type name into Candidate Name field and verify it suggest a list with candidates sharing the same first name.</t>
+  </si>
+  <si>
+    <t>Verify that after searching candidates with the same names it returns a list of candidates with the same names</t>
+  </si>
+  <si>
+    <t>When selecting one candidate it returns one record only</t>
+  </si>
+  <si>
+    <t>Verify candidate was added after inputing correct information into all required fields only.</t>
+  </si>
+  <si>
+    <t>1.
+2. 
+3.
+4.
+5.
+6.
+7.
+8.
+9</t>
+  </si>
+  <si>
+    <t>1. Open the application and successfully log in.
+2. Navigate to Recruitment page by clicking on side navigation panel.
+3. Click on "+ Add" button.
+4. In the "Add Candidate" window input data into 'First name', 'Middle name', 'Last name' and Email fields.
+5.Verify that date in the 'Date of Application' input field is current'
+6.Click on "Save" button
+7. Verify the toast message "Success Successfully Saved" poped up on the screen.
+8. Verify 'Application STage' header appeared and "Candidate History" section contains 1 record.
+9. Return to 'Recruitment' page and verify that created record was added to the list</t>
   </si>
 </sst>
 </file>
@@ -200,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -210,6 +244,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,17 +530,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -761,76 +799,88 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>22</v>
@@ -838,7 +888,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>23</v>
@@ -846,7 +896,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
@@ -854,29 +904,49 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">

</xml_diff>

<commit_message>
Recruitment page TCRP01 test case was updated. Some minor changes were done to selenium driver
</commit_message>
<xml_diff>
--- a/test_cases/OrangeHRM_test_cases.xlsx
+++ b/test_cases/OrangeHRM_test_cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4eto\pythonProject\orangehrm_demo_framework\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7280423-5896-4C01-9586-FB9ACC44DC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747F3BE8-B984-44FA-957A-554144B85B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -87,9 +87,6 @@
   <si>
     <t>UserName - "Admin"
 Password - "adme321"</t>
-  </si>
-  <si>
-    <t>Test cases for Recruitment Page</t>
   </si>
   <si>
     <t>Side navigation panel</t>
@@ -199,6 +196,16 @@
 7. Verify the toast message "Success Successfully Saved" poped up on the screen.
 8. Verify 'Application STage' header appeared and "Candidate History" section contains 1 record.
 9. Return to 'Recruitment' page and verify that created record was added to the list</t>
+  </si>
+  <si>
+    <t>Firstname : Stan Lastname : Smith
+email: stan_smith@gmail.com</t>
+  </si>
+  <si>
+    <t>New record was successfully saved. Success toast message appeared.</t>
+  </si>
+  <si>
+    <t>Test cases for Recruitment Page (TCRP)</t>
   </si>
 </sst>
 </file>
@@ -234,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -246,7 +253,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,8 +550,8 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,211 +735,232 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="A32" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="A33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6" ht="195" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="A34" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="2"/>
+      <c r="E34" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -930,27 +970,27 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>

</xml_diff>

<commit_message>
Several method added to recruitment_page
</commit_message>
<xml_diff>
--- a/test_cases/OrangeHRM_test_cases.xlsx
+++ b/test_cases/OrangeHRM_test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4eto\pythonProject\orangehrm_demo_framework\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747F3BE8-B984-44FA-957A-554144B85B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27F59E5-BB30-49FB-8D68-E888B7285639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -116,12 +116,6 @@
     <t>Try to add new candidate with required fields filled in and future date</t>
   </si>
   <si>
-    <t>Try to add new candidate with required fields filled in and calendar date typed  in</t>
-  </si>
-  <si>
-    <t>Try to add new candidate with valid characters in required fields and date selected from calendar</t>
-  </si>
-  <si>
     <t>Verify that date in the calendar equals to current date when adding new candidate</t>
   </si>
   <si>
@@ -174,17 +168,6 @@
   </si>
   <si>
     <t>Verify candidate was added after inputing correct information into all required fields only.</t>
-  </si>
-  <si>
-    <t>1.
-2. 
-3.
-4.
-5.
-6.
-7.
-8.
-9</t>
   </si>
   <si>
     <t>1. Open the application and successfully log in.
@@ -206,6 +189,29 @@
   </si>
   <si>
     <t>Test cases for Recruitment Page (TCRP)</t>
+  </si>
+  <si>
+    <t>1. Open the application and successfully log in.
+2. Navigate to Recruitment page by clicking on side navigation panel.
+3. Click on "+ Add" button.
+4. In the "Add Candidate" window input data into 'First name', 'Middle name', 'Last name' and Email fields.5.
+6.
+7.
+8.
+9</t>
+  </si>
+  <si>
+    <t>Input date in incerrect format</t>
+  </si>
+  <si>
+    <t>Firstname : Adam Lastname : Smith
+email: stan_smith@gmail.com</t>
+  </si>
+  <si>
+    <t>Add new candidate with valid characters in required fields and date typed from calendar</t>
+  </si>
+  <si>
+    <t>Try to add new candidate with all fields filled in and calendar date typed  in</t>
   </si>
 </sst>
 </file>
@@ -241,16 +247,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -262,10 +262,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,8 +553,8 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,88 +739,88 @@
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="4"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="4"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="4"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="4"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="4"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="4"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -836,167 +839,209 @@
       <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6" ht="195" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="B36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Methods added to recruitment_page and tests added to recruitment_test
</commit_message>
<xml_diff>
--- a/test_cases/OrangeHRM_test_cases.xlsx
+++ b/test_cases/OrangeHRM_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4eto\pythonProject\orangehrm_demo_framework\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27F59E5-BB30-49FB-8D68-E888B7285639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BCF350-28B5-43C0-875E-B7BF46A36A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>TCRP005</t>
-  </si>
-  <si>
-    <t>TCRP006</t>
   </si>
   <si>
     <t>TCRP007</t>
@@ -212,6 +209,21 @@
   </si>
   <si>
     <t>Try to add new candidate with all fields filled in and calendar date typed  in</t>
+  </si>
+  <si>
+    <t>vacancy: Associate IT Manager</t>
+  </si>
+  <si>
+    <t>TCRP00602</t>
+  </si>
+  <si>
+    <t>TCRP00601</t>
+  </si>
+  <si>
+    <t>first_name="Steven", last_name="Jonson", email="sjonson@gmail.com", middle_name="Jeremy", contact_number="(999) 123-45-67", vacancy_name="Senior QA Lead", keywords="associate, it, manager", date="2022-09-01", notes="Test test test", consent="v"</t>
+  </si>
+  <si>
+    <t>cycle of candidate - initiated, shortlisted, schedule interview, hired , rejected</t>
   </si>
 </sst>
 </file>
@@ -550,11 +562,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +832,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -843,16 +855,16 @@
         <v>30</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="F34" s="4"/>
     </row>
@@ -861,13 +873,13 @@
         <v>31</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="2"/>
@@ -880,7 +892,7 @@
         <v>27</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -894,7 +906,7 @@
         <v>29</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -908,7 +920,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -916,41 +928,45 @@
     </row>
     <row r="39" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E40" s="3"/>
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -958,13 +974,13 @@
     </row>
     <row r="42" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -972,13 +988,13 @@
     </row>
     <row r="43" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -986,69 +1002,88 @@
     </row>
     <row r="44" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="B45" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>41</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A61:F61"/>
     <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A49:F49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated README.md file and test_cases file
</commit_message>
<xml_diff>
--- a/test_cases/OrangeHRM_test_cases.xlsx
+++ b/test_cases/OrangeHRM_test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4eto\pythonProject\orangehrm_demo_framework\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D339B2-F1D2-45AC-9999-57179F5DA796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666C40C9-BA78-487E-A3EF-25B4055E3192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="570" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Test Case description</t>
   </si>
@@ -182,6 +182,36 @@
   </si>
   <si>
     <t>Recruitment</t>
+  </si>
+  <si>
+    <t>TS_OHRM_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Recruitment page Candidates tab functionality </t>
+  </si>
+  <si>
+    <t>TC_OHRM_RPCT_001</t>
+  </si>
+  <si>
+    <t>Add candidate with correct required data only</t>
+  </si>
+  <si>
+    <t>FirstName - "Stan"
+LastName - "Smith" 
+Email - "stan_smith@gmail.com"</t>
+  </si>
+  <si>
+    <t>1. Successfully login to the app
+2. Click on 'Recruitment' menu on the side pannel
+3. Verify location is 'Candidates' tab
+4. Verify there is no record with Test Data details in the 'Records Found' section on the page
+5. Click 'Add' button
+6. On the appeared form input Test Data (FirstName, LastName, Email) and click 'Save' button.
+7. Verify record with Test Data details appeared on the 'Records Found' section on the page.</t>
+  </si>
+  <si>
+    <t>Success' green toast message should appear and Candidate profile should be on the screen after saving.
+The record with Test Data details should appear on the 'Records Found' section on the page.</t>
   </si>
 </sst>
 </file>
@@ -329,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -358,6 +388,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,9 +674,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,14 +901,28 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+    <row r="11" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -899,74 +946,74 @@
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="1"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="1"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="1"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="1"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="1"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="1"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="1"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>

</xml_diff>